<commit_message>
Virtual Trading Logs Update
</commit_message>
<xml_diff>
--- a/testers/5-real_world_application/VirtualTradingLogs.xlsx
+++ b/testers/5-real_world_application/VirtualTradingLogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ACD\SP\OLARTE_SP\testers\5-real_world_application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48FB881B-C34D-4063-8BBF-B4A98E9127D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC3FEA88-2E2C-4D44-BEC6-B6EFC1B87442}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Stocks</t>
   </si>
@@ -272,6 +272,24 @@
   </si>
   <si>
     <t>BLOOM</t>
+  </si>
+  <si>
+    <t>MPI</t>
+  </si>
+  <si>
+    <t>TEL</t>
+  </si>
+  <si>
+    <t>GLO</t>
+  </si>
+  <si>
+    <t>JGS</t>
+  </si>
+  <si>
+    <t>BDO</t>
+  </si>
+  <si>
+    <t>FGEN</t>
   </si>
 </sst>
 </file>
@@ -363,7 +381,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -381,6 +399,8 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -388,7 +408,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -669,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,7 +701,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="6" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
     <col min="9" max="9" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
@@ -691,29 +710,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
@@ -765,9 +784,15 @@
       <c r="E3" s="8">
         <v>5006.4799999999996</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0</v>
+      </c>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -790,9 +815,15 @@
       <c r="E4" s="4">
         <v>0</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>10079.65</v>
+      </c>
+      <c r="H4" s="7">
+        <v>9960.0499999999993</v>
+      </c>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
@@ -815,9 +846,15 @@
       <c r="E5" s="8">
         <v>15336.5</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>15345.14</v>
+      </c>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
@@ -840,9 +877,15 @@
       <c r="E6" s="4">
         <v>0</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="F6" s="5">
+        <v>7343.5</v>
+      </c>
+      <c r="G6" s="7">
+        <v>7103.5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>7053.45</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -862,12 +905,18 @@
       <c r="D7" s="8">
         <v>5523.28</v>
       </c>
-      <c r="E7" s="14">
-        <v>5473.22</v>
-      </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="E7" s="11">
+        <v>5428.21</v>
+      </c>
+      <c r="F7" s="7">
+        <v>5344.39</v>
+      </c>
+      <c r="G7" s="7">
+        <v>5394.08</v>
+      </c>
+      <c r="H7" s="8">
+        <v>6964.37</v>
+      </c>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -890,9 +939,15 @@
       <c r="E8" s="4">
         <v>0</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>7173.47</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -915,9 +970,15 @@
       <c r="E9" s="8">
         <v>31961.360000000001</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="F9" s="5">
+        <v>32144.55</v>
+      </c>
+      <c r="G9" s="7">
+        <v>31242.85</v>
+      </c>
+      <c r="H9" s="7">
+        <v>30920.76</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -940,9 +1001,15 @@
       <c r="E10" s="8">
         <v>2710.69</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2722.81</v>
+      </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -956,15 +1023,29 @@
       <c r="B11">
         <v>500</v>
       </c>
-      <c r="C11" s="13">
-        <v>0</v>
-      </c>
-      <c r="D11" s="13">
+      <c r="C11" s="4">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
         <v>0</v>
       </c>
       <c r="E11" s="5">
         <v>14191.74</v>
       </c>
+      <c r="F11" s="8">
+        <v>13949.03</v>
+      </c>
+      <c r="G11" s="5">
+        <v>13379.18</v>
+      </c>
+      <c r="H11" s="7">
+        <v>13106.64</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -973,121 +1054,365 @@
       <c r="B12">
         <v>500</v>
       </c>
-      <c r="C12" s="13">
-        <v>0</v>
-      </c>
-      <c r="D12" s="13">
+      <c r="C12" s="4">
+        <v>0</v>
+      </c>
+      <c r="D12" s="4">
         <v>0</v>
       </c>
       <c r="E12" s="5">
         <v>4643.09</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="F12" s="7">
+        <v>4479.74</v>
+      </c>
+      <c r="G12" s="7">
+        <v>4469.8</v>
+      </c>
+      <c r="H12" s="7">
+        <v>4469.8</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13">
+        <v>5000</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>21011.8</v>
+      </c>
+      <c r="G13" s="7">
+        <v>20167.87</v>
+      </c>
+      <c r="H13" s="7">
+        <v>20019.21</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="12">
+        <v>25</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0</v>
+      </c>
+      <c r="D14" s="4">
+        <v>0</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <v>32094.400000000001</v>
+      </c>
+      <c r="H14" s="8">
+        <v>32605.55</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="12">
+        <v>25</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <v>45132.75</v>
+      </c>
+      <c r="H15" s="7">
+        <v>45092.78</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="12">
+        <v>50</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0</v>
+      </c>
+      <c r="G16" s="15">
+        <v>0</v>
+      </c>
+      <c r="H16" s="5">
+        <v>6233.33</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+    </row>
+    <row r="17" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="12">
+        <v>50</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0</v>
+      </c>
+      <c r="G17" s="15">
+        <v>0</v>
+      </c>
+      <c r="H17" s="5">
+        <v>2572.7800000000002</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="9"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+    <row r="18" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="12">
+        <v>500</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4">
+        <v>0</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0</v>
+      </c>
+      <c r="G18" s="15">
+        <v>0</v>
+      </c>
+      <c r="H18" s="5">
+        <v>8494.99</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="4">
-        <v>49601.74</v>
-      </c>
-      <c r="D20" s="4">
-        <v>43962.75</v>
-      </c>
-      <c r="E20" s="4">
-        <v>80142.95</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="C20" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
-      <c r="B21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4">
-        <v>50398.26</v>
-      </c>
-      <c r="D21" s="4">
-        <v>55049.53</v>
-      </c>
-      <c r="E21" s="4">
-        <v>18592.54</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="4">
-        <f>SUM(C20,C21)</f>
-        <v>100000</v>
-      </c>
-      <c r="D22" s="4">
-        <f>SUM(D20,D21)</f>
-        <v>99012.28</v>
-      </c>
-      <c r="E22" s="4">
-        <f>SUM(E20:E21)</f>
-        <v>98735.489999999991</v>
-      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="9"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="4"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="4">
+        <f>49601.74+100000</f>
+        <v>149601.74</v>
+      </c>
+      <c r="D25" s="4">
+        <f>43962.75+100000</f>
+        <v>143962.75</v>
+      </c>
+      <c r="E25" s="4">
+        <f>80142.95+100000</f>
+        <v>180142.95</v>
+      </c>
+      <c r="F25" s="4">
+        <f>28163.92+100000</f>
+        <v>128163.92</v>
+      </c>
+      <c r="G25" s="4">
+        <f>22772.85+4544.45</f>
+        <v>27317.3</v>
+      </c>
+      <c r="H25" s="4">
+        <f>12835.88+9948.82</f>
+        <v>22784.699999999997</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="4">
+        <f>50398.26</f>
+        <v>50398.26</v>
+      </c>
+      <c r="D26" s="4">
+        <f>55049.53</f>
+        <v>55049.53</v>
+      </c>
+      <c r="E26" s="4">
+        <v>18592.54</v>
+      </c>
+      <c r="F26" s="4">
+        <v>69602.36</v>
+      </c>
+      <c r="G26" s="4">
+        <f>91717.34+76310.85</f>
+        <v>168028.19</v>
+      </c>
+      <c r="H26" s="4">
+        <f>85440.83+87055.98</f>
+        <v>172496.81</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+      <c r="M26" s="2"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="4">
+        <f>SUM(C25,C26)</f>
+        <v>200000</v>
+      </c>
+      <c r="D27" s="4">
+        <f>SUM(D25,D26)</f>
+        <v>199012.28</v>
+      </c>
+      <c r="E27" s="4">
+        <f>SUM(E25:E26)</f>
+        <v>198735.49000000002</v>
+      </c>
+      <c r="F27" s="4">
+        <f>SUM(F25:F26)</f>
+        <v>197766.28</v>
+      </c>
+      <c r="G27" s="4">
+        <f>SUM(G25:G26)</f>
+        <v>195345.49</v>
+      </c>
+      <c r="H27" s="4">
+        <f>SUM(H25:H26)</f>
+        <v>195281.51</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Updated Logs for Test#5
</commit_message>
<xml_diff>
--- a/testers/5-real_world_application/VirtualTradingLogs.xlsx
+++ b/testers/5-real_world_application/VirtualTradingLogs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ACD\SP\OLARTE_SP\testers\5-real_world_application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A08C94A-B5B5-474C-B866-35F36CDD6BF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726956E-0D3C-4D60-882F-9F689E3EB0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34785" yWindow="-4710" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Stocks</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>FGEN</t>
-  </si>
-  <si>
-    <t>PSEI</t>
   </si>
   <si>
     <t>ICT</t>
@@ -339,7 +336,7 @@
     <numFmt numFmtId="164" formatCode="&quot;₱&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,6 +380,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFF7F9F9"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -416,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -446,15 +449,22 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="4" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -737,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,59 +768,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
       <c r="C2" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="J2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="M2" s="9" t="s">
         <v>35</v>
-      </c>
-      <c r="M2" s="9" t="s">
-        <v>36</v>
       </c>
       <c r="N2" s="1"/>
     </row>
@@ -822,10 +832,12 @@
       <c r="C3" s="6">
         <v>10380.530000000001</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <v>9910.5</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="17">
+        <v>10079.65</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -843,10 +855,12 @@
       <c r="C4" s="6">
         <v>2645.29</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="17">
         <v>2572.7800000000002</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="24">
+        <v>2501.98</v>
+      </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -862,10 +876,12 @@
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="19">
+      <c r="D5" s="17">
         <v>6348.35</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="17">
+        <v>6298.34</v>
+      </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -883,10 +899,12 @@
       <c r="C6" s="6">
         <v>8174.04</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D6" s="18">
         <v>8146.43</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="17">
+        <v>8244.25</v>
+      </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -898,7 +916,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="13"/>
       <c r="C7" s="3"/>
@@ -921,10 +939,12 @@
       <c r="C8" s="6">
         <v>14292.04</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="17">
         <v>14292.04</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="24">
+        <v>14097.69</v>
+      </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -940,10 +960,12 @@
       </c>
       <c r="B9" s="13"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="19">
+      <c r="D9" s="17">
         <v>5303.19</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="17">
+        <v>5273.19</v>
+      </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -961,10 +983,12 @@
       <c r="C10" s="6">
         <v>33849.56</v>
       </c>
-      <c r="D10" s="20">
+      <c r="D10" s="18">
         <v>32977.19</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="17">
+        <v>34300.89</v>
+      </c>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -982,10 +1006,12 @@
       <c r="C11" s="6">
         <v>46386.44</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="17">
         <v>45659.3</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="24">
+        <v>45836.06</v>
+      </c>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -1001,10 +1027,12 @@
       </c>
       <c r="B12" s="13"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="19">
+      <c r="D12" s="17">
         <v>4573.08</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="24">
+        <v>4574.16</v>
+      </c>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1033,14 +1061,16 @@
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B14" s="13"/>
       <c r="C14" s="3"/>
-      <c r="D14" s="19">
+      <c r="D14" s="17">
         <v>14943.96</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="17">
+        <v>15365.19</v>
+      </c>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1058,10 +1088,12 @@
       <c r="C15" s="6">
         <v>33398.239999999998</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="17">
         <v>33348.089999999997</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="24">
+        <v>32977.19</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1079,10 +1111,12 @@
       <c r="C16" s="6">
         <v>16398.23</v>
       </c>
-      <c r="D16" s="20">
+      <c r="D16" s="18">
         <v>16203.67</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="17">
+        <v>16548.68</v>
+      </c>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -1100,10 +1134,10 @@
       <c r="C17" s="6">
         <v>5018.1499999999996</v>
       </c>
-      <c r="D17" s="20">
+      <c r="D17" s="18">
         <v>4966.7299999999996</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -1121,10 +1155,12 @@
       <c r="C18" s="6">
         <v>18203.54</v>
       </c>
-      <c r="D18" s="20">
+      <c r="D18" s="18">
         <v>18185.77</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="17">
+        <v>19156.349999999999</v>
+      </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -1136,16 +1172,16 @@
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="6">
         <v>18429.21</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="18">
         <v>18379.060000000001</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1180,7 +1216,7 @@
       <c r="C21" s="6">
         <v>7363.5</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="18">
         <v>7262.52</v>
       </c>
       <c r="E21" s="3"/>
@@ -1194,12 +1230,10 @@
       <c r="M21" s="3"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="22"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1255,7 +1289,9 @@
       <c r="D28" s="3">
         <v>737694.19</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="3">
+        <v>722414.73</v>
+      </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -1282,7 +1318,9 @@
       <c r="D29" s="3">
         <v>256508.16</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3">
+        <v>272672.12</v>
+      </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -1310,7 +1348,10 @@
         <f>SUM(D28:D29)</f>
         <v>994202.35</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="3">
+        <f>SUM(E28:E29)</f>
+        <v>995086.85</v>
+      </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -1328,7 +1369,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" s="15">
         <f>((D30-C30)/(C30))*100</f>
@@ -1336,11 +1377,11 @@
       </c>
       <c r="E31" s="15">
         <f t="shared" ref="E31:M31" si="0">((E30-D30)/(D30))*100</f>
+        <v>8.8965792527044424E-2</v>
+      </c>
+      <c r="F31" s="15">
+        <f t="shared" si="0"/>
         <v>-100</v>
-      </c>
-      <c r="F31" s="15" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
       </c>
       <c r="G31" s="15" t="e">
         <f t="shared" si="0"/>
@@ -1373,47 +1414,53 @@
     </row>
     <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="19">
+        <v>-1.29E-2</v>
+      </c>
+      <c r="E32" s="19">
+        <v>-1.06E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="25">
+        <v>165565.73000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D32" s="21">
-        <v>-1.1000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
-        <v>40</v>
       </c>
       <c r="C36" s="12">
         <v>1000000</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" t="s">
         <v>41</v>
       </c>
-      <c r="C37" t="s">
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
-        <v>43</v>
-      </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Test Logs for Test#5
</commit_message>
<xml_diff>
--- a/testers/5-real_world_application/VirtualTradingLogs.xlsx
+++ b/testers/5-real_world_application/VirtualTradingLogs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\ACD\SP\OLARTE_SP\testers\5-real_world_application\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF22EBF9-608D-46C2-B81C-2002677FD396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F45E70-66F3-43E9-BF95-156B944CD5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10140" yWindow="0" windowWidth="10455" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>Stocks</t>
   </si>
@@ -266,6 +266,22 @@
     </r>
   </si>
   <si>
+    <t>Action Legends</t>
+  </si>
+  <si>
+    <t>Sold</t>
+  </si>
+  <si>
+    <t>Bought</t>
+  </si>
+  <si>
+    <t>Gain (%)</t>
+  </si>
+  <si>
+    <t>Baseline
+(PSEI)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">9 
 </t>
@@ -279,7 +295,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(April 6, 2023)</t>
+      <t>(April 11, 2023)</t>
     </r>
   </si>
   <si>
@@ -296,24 +312,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(April 7, 2023)</t>
-    </r>
-  </si>
-  <si>
-    <t>Action Legends</t>
-  </si>
-  <si>
-    <t>Sold</t>
-  </si>
-  <si>
-    <t>Bought</t>
-  </si>
-  <si>
-    <t>Gain (%)</t>
-  </si>
-  <si>
-    <t>Baseline
-(PSEI)</t>
+      <t>(April 12, 2023)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -738,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0">
+      <selection activeCell="AV56" sqref="AV56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -754,7 +754,7 @@
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
     <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="11.85546875" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -808,10 +808,10 @@
         <v>33</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="N2" s="1"/>
     </row>
@@ -837,8 +837,13 @@
       <c r="I3" s="7"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="17">
+        <v>10179.94</v>
+      </c>
       <c r="M3" s="3"/>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -866,8 +871,13 @@
       <c r="K4" s="18">
         <v>2497.0100000000002</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="17">
+        <v>24572.28</v>
+      </c>
       <c r="M4" s="3"/>
+      <c r="N4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -893,8 +903,13 @@
       <c r="K5" s="18">
         <v>6149.41</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="17">
+        <v>6523.38</v>
+      </c>
       <c r="M5" s="3"/>
+      <c r="N5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -922,8 +937,13 @@
       <c r="K6" s="18">
         <v>8195.98</v>
       </c>
-      <c r="L6" s="3"/>
+      <c r="L6" s="17">
+        <v>8294.4</v>
+      </c>
       <c r="M6" s="3"/>
+      <c r="N6" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -941,8 +961,13 @@
       <c r="K7" s="17">
         <v>10530.98</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="17">
+        <v>10530.98</v>
+      </c>
       <c r="M7" s="3"/>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -974,8 +999,13 @@
       <c r="K8" s="18">
         <v>13726.04</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="17">
+        <v>13690.27</v>
+      </c>
       <c r="M8" s="3"/>
+      <c r="N8" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1001,8 +1031,13 @@
       <c r="K9" s="18">
         <v>5225.13</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="17">
+        <v>5298.19</v>
+      </c>
       <c r="M9" s="3"/>
+      <c r="N9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1032,8 +1067,13 @@
       <c r="K10" s="17">
         <v>32119.47</v>
       </c>
-      <c r="L10" s="3"/>
+      <c r="L10" s="18">
+        <v>30995.09</v>
+      </c>
       <c r="M10" s="3"/>
+      <c r="N10" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1057,8 +1097,10 @@
       <c r="I11" s="7"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
       <c r="M11" s="3"/>
+      <c r="N11" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1084,6 +1126,9 @@
       </c>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1099,8 +1144,13 @@
       <c r="I13" s="7"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="17">
+        <v>7473.52</v>
+      </c>
       <c r="M13" s="3"/>
+      <c r="N13" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
@@ -1128,9 +1178,13 @@
       <c r="K14" s="17">
         <v>15545.73</v>
       </c>
-      <c r="L14" s="3"/>
+      <c r="L14" s="17">
+        <v>15846.61</v>
+      </c>
       <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
+      <c r="N14" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
@@ -1158,9 +1212,13 @@
       <c r="K15" s="17">
         <v>32595.88</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="17">
+        <v>32445.43</v>
+      </c>
       <c r="M15" s="3"/>
-      <c r="N15" s="3"/>
+      <c r="N15" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
@@ -1192,9 +1250,13 @@
       <c r="K16" s="18">
         <v>16302.77</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="17">
+        <v>16222.72</v>
+      </c>
       <c r="M16" s="3"/>
-      <c r="N16" s="3"/>
+      <c r="N16" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
@@ -1227,9 +1289,13 @@
       <c r="K17" s="18">
         <v>4946.8500000000004</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="18">
+        <v>4936.91</v>
+      </c>
       <c r="M17" s="3"/>
-      <c r="N17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -1263,7 +1329,9 @@
       </c>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="3"/>
+      <c r="N18" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="19" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
@@ -1287,9 +1355,13 @@
       </c>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
+      <c r="L19" s="17">
+        <v>18805.310000000001</v>
+      </c>
       <c r="M19" s="3"/>
-      <c r="N19" s="3"/>
+      <c r="N19" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1315,9 +1387,13 @@
       <c r="K20" s="18">
         <v>2670.93</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="17">
+        <v>2697.8</v>
+      </c>
       <c r="M20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="N20" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
@@ -1341,9 +1417,10 @@
       <c r="K21" s="17">
         <v>7073.46</v>
       </c>
-      <c r="L21" s="3"/>
       <c r="M21" s="3"/>
-      <c r="N21" s="3"/>
+      <c r="N21" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
@@ -1426,7 +1503,9 @@
       <c r="K28" s="3">
         <v>717688.51</v>
       </c>
-      <c r="L28" s="3"/>
+      <c r="L28" s="3">
+        <v>581039.69999999995</v>
+      </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -1467,7 +1546,9 @@
       <c r="K29" s="3">
         <v>270295.53000000003</v>
       </c>
-      <c r="L29" s="3"/>
+      <c r="L29" s="3">
+        <v>405709.37</v>
+      </c>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -1516,7 +1597,10 @@
         <f>SUM(K28:K29)</f>
         <v>987984.04</v>
       </c>
-      <c r="L30" s="3"/>
+      <c r="L30" s="3">
+        <f>SUM(L28:L29)</f>
+        <v>986749.07</v>
+      </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
@@ -1527,7 +1611,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C31" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D31" s="21">
         <f>((D30-C30)/(C30))*100</f>
@@ -1563,19 +1647,19 @@
       </c>
       <c r="L31" s="15">
         <f t="shared" si="1"/>
+        <v>-0.12499898277709914</v>
+      </c>
+      <c r="M31" s="16">
+        <f t="shared" si="1"/>
         <v>-100</v>
-      </c>
-      <c r="M31" s="16" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" s="23">
         <v>-1.29E-2</v>
@@ -1601,10 +1685,13 @@
       <c r="K32" s="23">
         <v>-9.2999999999999992E-3</v>
       </c>
+      <c r="L32" s="24">
+        <v>-1.32E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E33" s="20">
         <v>165565.73000000001</v>
@@ -1612,7 +1699,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>